<commit_message>
Eliminamos las carpetas externas y  agregamos Ca,Mg y P a la tabja metadata
</commit_message>
<xml_diff>
--- a/spectra/metadata.xlsx
+++ b/spectra/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\GitHub\trigo 2021\spectra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E95AD6CF-4768-4EB7-92FE-EF790DB59636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627B4B64-8399-4F2E-913D-4FB6698B8A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{89CF3514-2ED7-4E9D-82F5-8D6920B71450}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="50">
   <si>
     <t>W S -</t>
   </si>
@@ -127,13 +127,70 @@
   </si>
   <si>
     <t>Si</t>
+  </si>
+  <si>
+    <t>-27.59 u</t>
+  </si>
+  <si>
+    <t>-43.29 u</t>
+  </si>
+  <si>
+    <t>-8.40 u</t>
+  </si>
+  <si>
+    <t>6.67 u</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>Mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>-1.26 u</t>
+  </si>
+  <si>
+    <t>-1.94 u</t>
+  </si>
+  <si>
+    <t>-0.61 u</t>
+  </si>
+  <si>
+    <t>-0.23 u</t>
+  </si>
+  <si>
+    <t>-0.48 u</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>-8.03 u</t>
+  </si>
+  <si>
+    <t>-52.32 u</t>
+  </si>
+  <si>
+    <t>-59.03 u</t>
+  </si>
+  <si>
+    <t>-68.33 u</t>
+  </si>
+  <si>
+    <t>-63.74 u</t>
+  </si>
+  <si>
+    <t>-56.50 u</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +248,36 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -327,11 +414,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -413,10 +501,25 @@
     <xf numFmtId="37" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{40136762-5A0C-41F9-BDA7-F4B728A18ABE}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{EDEB1574-0328-4D2B-8120-AFA4984A6952}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -728,15 +831,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFE65F2-1C41-4C98-8A15-1B3EF8916CC0}">
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="G52" sqref="G51:G52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -752,8 +855,17 @@
       <c r="E1" s="32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="14">
         <v>125</v>
       </c>
@@ -769,8 +881,18 @@
       <c r="E2" s="27">
         <v>2884.61</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F2" s="33">
+        <v>3519.81</v>
+      </c>
+      <c r="G2" s="36">
+        <v>694.76</v>
+      </c>
+      <c r="H2" s="40">
+        <v>837.54</v>
+      </c>
+      <c r="I2" s="35"/>
+    </row>
+    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="14">
         <v>126</v>
       </c>
@@ -786,8 +908,18 @@
       <c r="E3" s="27">
         <v>4623.33</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F3" s="33">
+        <v>3134.65</v>
+      </c>
+      <c r="G3" s="36">
+        <v>582.64</v>
+      </c>
+      <c r="H3" s="40">
+        <v>720.58</v>
+      </c>
+      <c r="I3" s="35"/>
+    </row>
+    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="14">
         <v>127</v>
       </c>
@@ -803,8 +935,18 @@
       <c r="E4" s="27">
         <v>1718.91</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F4" s="33">
+        <v>2473.7399999999998</v>
+      </c>
+      <c r="G4" s="36">
+        <v>462.32</v>
+      </c>
+      <c r="H4" s="40">
+        <v>375.33</v>
+      </c>
+      <c r="I4" s="35"/>
+    </row>
+    <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <v>128</v>
       </c>
@@ -820,8 +962,18 @@
       <c r="E5" s="27">
         <v>2698.15</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F5" s="33">
+        <v>4743.0200000000004</v>
+      </c>
+      <c r="G5" s="36">
+        <v>876.45</v>
+      </c>
+      <c r="H5" s="40">
+        <v>666.59</v>
+      </c>
+      <c r="I5" s="35"/>
+    </row>
+    <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <v>129</v>
       </c>
@@ -837,8 +989,18 @@
       <c r="E6" s="27">
         <v>5348.13</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F6" s="33">
+        <v>4726.84</v>
+      </c>
+      <c r="G6" s="36">
+        <v>752.08</v>
+      </c>
+      <c r="H6" s="40">
+        <v>683.11</v>
+      </c>
+      <c r="I6" s="35"/>
+    </row>
+    <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <v>130</v>
       </c>
@@ -854,8 +1016,18 @@
       <c r="E7" s="27">
         <v>6683.08</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="33">
+        <v>4738.43</v>
+      </c>
+      <c r="G7" s="36">
+        <v>857.63</v>
+      </c>
+      <c r="H7" s="40">
+        <v>1053.96</v>
+      </c>
+      <c r="I7" s="35"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>131</v>
       </c>
@@ -869,8 +1041,19 @@
       <c r="E8" s="28">
         <v>22196.1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F8" s="33">
+        <v>1294.69</v>
+      </c>
+      <c r="G8" s="36">
+        <v>303.85000000000002</v>
+      </c>
+      <c r="H8" s="40">
+        <v>40.56</v>
+      </c>
+      <c r="I8" s="38"/>
+      <c r="J8" s="42"/>
+    </row>
+    <row r="9" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="14">
         <v>132</v>
       </c>
@@ -886,8 +1069,18 @@
       <c r="E9" s="27">
         <v>6571.77</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F9" s="33">
+        <v>1105.48</v>
+      </c>
+      <c r="G9" s="36">
+        <v>399.03</v>
+      </c>
+      <c r="H9" s="40">
+        <v>25.41</v>
+      </c>
+      <c r="I9" s="35"/>
+    </row>
+    <row r="10" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="14">
         <v>133</v>
       </c>
@@ -903,8 +1096,18 @@
       <c r="E10" s="27">
         <v>9901.81</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F10" s="33">
+        <v>1792.21</v>
+      </c>
+      <c r="G10" s="36">
+        <v>516.25</v>
+      </c>
+      <c r="H10" s="40">
+        <v>50.27</v>
+      </c>
+      <c r="I10" s="35"/>
+    </row>
+    <row r="11" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="14">
         <v>134</v>
       </c>
@@ -920,8 +1123,18 @@
       <c r="E11" s="28">
         <v>17727.28</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F11" s="33">
+        <v>1071.45</v>
+      </c>
+      <c r="G11" s="36">
+        <v>332.04</v>
+      </c>
+      <c r="H11" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" s="35"/>
+    </row>
+    <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="16">
         <v>135</v>
       </c>
@@ -937,8 +1150,18 @@
       <c r="E12" s="27">
         <v>13841.8</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F12" s="33">
+        <v>4508.18</v>
+      </c>
+      <c r="G12" s="36">
+        <v>898.48</v>
+      </c>
+      <c r="H12" s="40">
+        <v>768.83</v>
+      </c>
+      <c r="I12" s="41"/>
+    </row>
+    <row r="13" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="16">
         <v>136</v>
       </c>
@@ -954,8 +1177,18 @@
       <c r="E13" s="27">
         <v>13443.67</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F13" s="33">
+        <v>3006.45</v>
+      </c>
+      <c r="G13" s="36">
+        <v>720.26</v>
+      </c>
+      <c r="H13" s="40">
+        <v>221.89</v>
+      </c>
+      <c r="I13" s="35"/>
+    </row>
+    <row r="14" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="16">
         <v>137</v>
       </c>
@@ -971,8 +1204,18 @@
       <c r="E14" s="28">
         <v>41892.519999999997</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F14" s="33">
+        <v>3396.71</v>
+      </c>
+      <c r="G14" s="36">
+        <v>738.38</v>
+      </c>
+      <c r="H14" s="40">
+        <v>276.95999999999998</v>
+      </c>
+      <c r="I14" s="35"/>
+    </row>
+    <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <v>138</v>
       </c>
@@ -988,8 +1231,18 @@
       <c r="E15" s="27">
         <v>695.35</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F15" s="33">
+        <v>3312.31</v>
+      </c>
+      <c r="G15" s="36">
+        <v>638.46</v>
+      </c>
+      <c r="H15" s="40">
+        <v>1127.6199999999999</v>
+      </c>
+      <c r="I15" s="35"/>
+    </row>
+    <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <v>139</v>
       </c>
@@ -1005,8 +1258,18 @@
       <c r="E16" s="27">
         <v>1336.68</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F16" s="33">
+        <v>6768.92</v>
+      </c>
+      <c r="G16" s="36">
+        <v>1080.4100000000001</v>
+      </c>
+      <c r="H16" s="40">
+        <v>1923.11</v>
+      </c>
+      <c r="I16" s="35"/>
+    </row>
+    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <v>140</v>
       </c>
@@ -1022,15 +1285,26 @@
       <c r="E17" s="27">
         <v>4358.49</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="33">
+        <v>2355.9499999999998</v>
+      </c>
+      <c r="G17" s="36">
+        <v>415.89</v>
+      </c>
+      <c r="H17" s="40">
+        <v>1059.72</v>
+      </c>
+      <c r="I17" s="35"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="1"/>
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
       <c r="E18" s="27"/>
-    </row>
-    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="I18" s="39"/>
+    </row>
+    <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="17">
         <v>141</v>
       </c>
@@ -1046,8 +1320,18 @@
       <c r="E19" s="27">
         <v>3800.27</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F19" s="33">
+        <v>1616.88</v>
+      </c>
+      <c r="G19" s="36">
+        <v>336.08</v>
+      </c>
+      <c r="H19" s="40">
+        <v>147.78</v>
+      </c>
+      <c r="I19" s="35"/>
+    </row>
+    <row r="20" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="14">
         <v>142</v>
       </c>
@@ -1063,8 +1347,18 @@
       <c r="E20" s="27">
         <v>3958.44</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F20" s="33">
+        <v>1750.3</v>
+      </c>
+      <c r="G20" s="36">
+        <v>337.72</v>
+      </c>
+      <c r="H20" s="40">
+        <v>240.95</v>
+      </c>
+      <c r="I20" s="35"/>
+    </row>
+    <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="14">
         <v>143</v>
       </c>
@@ -1080,8 +1374,18 @@
       <c r="E21" s="29">
         <v>11974.14</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F21" s="33">
+        <v>1550.87</v>
+      </c>
+      <c r="G21" s="36">
+        <v>364.47</v>
+      </c>
+      <c r="H21" s="40">
+        <v>149.46</v>
+      </c>
+      <c r="I21" s="35"/>
+    </row>
+    <row r="22" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <v>144</v>
       </c>
@@ -1097,8 +1401,18 @@
       <c r="E22" s="27">
         <v>10495.24</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F22" s="33">
+        <v>7536.23</v>
+      </c>
+      <c r="G22" s="36">
+        <v>1108.55</v>
+      </c>
+      <c r="H22" s="40">
+        <v>2601.0700000000002</v>
+      </c>
+      <c r="I22" s="35"/>
+    </row>
+    <row r="23" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <v>145</v>
       </c>
@@ -1114,8 +1428,18 @@
       <c r="E23" s="27">
         <v>11059.27</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F23" s="33">
+        <v>7521.79</v>
+      </c>
+      <c r="G23" s="36">
+        <v>1074.3399999999999</v>
+      </c>
+      <c r="H23" s="40">
+        <v>3313.07</v>
+      </c>
+      <c r="I23" s="35"/>
+    </row>
+    <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <v>146</v>
       </c>
@@ -1131,8 +1455,18 @@
       <c r="E24" s="28">
         <v>31423.43</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F24" s="33">
+        <v>6410.2</v>
+      </c>
+      <c r="G24" s="36">
+        <v>987.2</v>
+      </c>
+      <c r="H24" s="40">
+        <v>2674.28</v>
+      </c>
+      <c r="I24" s="35"/>
+    </row>
+    <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A25" s="18">
         <v>147</v>
       </c>
@@ -1148,8 +1482,18 @@
       <c r="E25" s="27">
         <v>2969.93</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F25" s="33">
+        <v>5326.18</v>
+      </c>
+      <c r="G25" s="36">
+        <v>573.16</v>
+      </c>
+      <c r="H25" s="40">
+        <v>1922.22</v>
+      </c>
+      <c r="I25" s="35"/>
+    </row>
+    <row r="26" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="18">
         <v>148</v>
       </c>
@@ -1165,8 +1509,18 @@
       <c r="E26" s="27">
         <v>2994.42</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F26" s="33">
+        <v>4475.38</v>
+      </c>
+      <c r="G26" s="36">
+        <v>401.19</v>
+      </c>
+      <c r="H26" s="40">
+        <v>1109.82</v>
+      </c>
+      <c r="I26" s="35"/>
+    </row>
+    <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A27" s="18">
         <v>149</v>
       </c>
@@ -1182,8 +1536,18 @@
       <c r="E27" s="29">
         <v>4026.41</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="33">
+        <v>3898.86</v>
+      </c>
+      <c r="G27" s="36">
+        <v>496.89</v>
+      </c>
+      <c r="H27" s="40">
+        <v>1281.9100000000001</v>
+      </c>
+      <c r="I27" s="35"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>159</v>
       </c>
@@ -1197,8 +1561,18 @@
       <c r="E28" s="28">
         <v>22872.78</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F28" s="33">
+        <v>1210.72</v>
+      </c>
+      <c r="G28" s="36">
+        <v>163.68</v>
+      </c>
+      <c r="H28" s="40">
+        <v>25.77</v>
+      </c>
+      <c r="I28" s="38"/>
+    </row>
+    <row r="29" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A29" s="17">
         <v>160</v>
       </c>
@@ -1214,8 +1588,18 @@
       <c r="E29" s="27">
         <v>7286.67</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F29" s="33">
+        <v>2387.61</v>
+      </c>
+      <c r="G29" s="36">
+        <v>226.01</v>
+      </c>
+      <c r="H29" s="40">
+        <v>425.97</v>
+      </c>
+      <c r="I29" s="35"/>
+    </row>
+    <row r="30" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="14">
         <v>161</v>
       </c>
@@ -1225,8 +1609,9 @@
       <c r="C30" s="25"/>
       <c r="D30" s="25"/>
       <c r="E30" s="27"/>
-    </row>
-    <row r="31" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="I30" s="39"/>
+    </row>
+    <row r="31" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A31" s="14">
         <v>162</v>
       </c>
@@ -1242,8 +1627,18 @@
       <c r="E31" s="28">
         <v>23947.67</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F31" s="33">
+        <v>2581.29</v>
+      </c>
+      <c r="G31" s="36">
+        <v>210.27</v>
+      </c>
+      <c r="H31" s="40">
+        <v>666.75</v>
+      </c>
+      <c r="I31" s="35"/>
+    </row>
+    <row r="32" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A32" s="15">
         <v>163</v>
       </c>
@@ -1259,8 +1654,18 @@
       <c r="E32" s="28">
         <v>21724.62</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F32" s="33">
+        <v>12406.99</v>
+      </c>
+      <c r="G32" s="36">
+        <v>1106.96</v>
+      </c>
+      <c r="H32" s="40">
+        <v>1117.3900000000001</v>
+      </c>
+      <c r="I32" s="35"/>
+    </row>
+    <row r="33" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <v>164</v>
       </c>
@@ -1270,8 +1675,9 @@
       <c r="C33" s="25"/>
       <c r="D33" s="25"/>
       <c r="E33" s="30"/>
-    </row>
-    <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="I33" s="39"/>
+    </row>
+    <row r="34" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <v>165</v>
       </c>
@@ -1287,8 +1693,18 @@
       <c r="E34" s="28">
         <v>64625.46</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F34" s="33">
+        <v>8875.02</v>
+      </c>
+      <c r="G34" s="36">
+        <v>632.35</v>
+      </c>
+      <c r="H34" s="40">
+        <v>678.83</v>
+      </c>
+      <c r="I34" s="35"/>
+    </row>
+    <row r="35" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="18">
         <v>166</v>
       </c>
@@ -1304,8 +1720,18 @@
       <c r="E35" s="27">
         <v>1440.49</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F35" s="33">
+        <v>25621.03</v>
+      </c>
+      <c r="G35" s="36">
+        <v>920.19</v>
+      </c>
+      <c r="H35" s="40">
+        <v>14991.18</v>
+      </c>
+      <c r="I35" s="35"/>
+    </row>
+    <row r="36" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A36" s="18">
         <v>167</v>
       </c>
@@ -1315,8 +1741,9 @@
       <c r="C36" s="25"/>
       <c r="D36" s="25"/>
       <c r="E36" s="27"/>
-    </row>
-    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="I36" s="39"/>
+    </row>
+    <row r="37" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A37" s="18">
         <v>168</v>
       </c>
@@ -1332,8 +1759,18 @@
       <c r="E37" s="29">
         <v>7179.45</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F37" s="33">
+        <v>24707.83</v>
+      </c>
+      <c r="G37" s="36">
+        <v>1722.84</v>
+      </c>
+      <c r="H37" s="40">
+        <v>16907.36</v>
+      </c>
+      <c r="I37" s="35"/>
+    </row>
+    <row r="38" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A38" s="19">
         <v>169</v>
       </c>
@@ -1349,8 +1786,18 @@
       <c r="E38" s="27">
         <v>1685.92</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F38" s="33">
+        <v>339.68</v>
+      </c>
+      <c r="G38" s="36">
+        <v>93.2</v>
+      </c>
+      <c r="H38" s="40">
+        <v>40.39</v>
+      </c>
+      <c r="I38" s="35"/>
+    </row>
+    <row r="39" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A39" s="19">
         <v>170</v>
       </c>
@@ -1360,8 +1807,9 @@
       <c r="C39" s="25"/>
       <c r="D39" s="25"/>
       <c r="E39" s="27"/>
-    </row>
-    <row r="40" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I39" s="39"/>
+    </row>
+    <row r="40" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="20">
         <v>171</v>
       </c>
@@ -1377,8 +1825,18 @@
       <c r="E40" s="29">
         <v>6336.04</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F40" s="33">
+        <v>1134.47</v>
+      </c>
+      <c r="G40" s="36">
+        <v>174.5</v>
+      </c>
+      <c r="H40" s="40">
+        <v>347.69</v>
+      </c>
+      <c r="I40" s="35"/>
+    </row>
+    <row r="41" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A41" s="17">
         <v>172</v>
       </c>
@@ -1394,8 +1852,18 @@
       <c r="E41" s="27">
         <v>7595.54</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F41" s="33">
+        <v>1464.72</v>
+      </c>
+      <c r="G41" s="36">
+        <v>135.16999999999999</v>
+      </c>
+      <c r="H41" s="40">
+        <v>201.08</v>
+      </c>
+      <c r="I41" s="35"/>
+    </row>
+    <row r="42" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A42" s="14">
         <v>173</v>
       </c>
@@ -1411,8 +1879,18 @@
       <c r="E42" s="28">
         <v>21184.06</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F42" s="33">
+        <v>1557.49</v>
+      </c>
+      <c r="G42" s="36">
+        <v>86.64</v>
+      </c>
+      <c r="H42" s="40">
+        <v>124.41</v>
+      </c>
+      <c r="I42" s="35"/>
+    </row>
+    <row r="43" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A43" s="14">
         <v>174</v>
       </c>
@@ -1428,8 +1906,18 @@
       <c r="E43" s="27">
         <v>10555.93</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F43" s="33">
+        <v>2870.53</v>
+      </c>
+      <c r="G43" s="36">
+        <v>159.71</v>
+      </c>
+      <c r="H43" s="40">
+        <v>144.27000000000001</v>
+      </c>
+      <c r="I43" s="35"/>
+    </row>
+    <row r="44" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <v>175</v>
       </c>
@@ -1445,8 +1933,18 @@
       <c r="E44" s="28">
         <v>18710.939999999999</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F44" s="33">
+        <v>5820.42</v>
+      </c>
+      <c r="G44" s="36">
+        <v>1055.72</v>
+      </c>
+      <c r="H44" s="40">
+        <v>2285.9899999999998</v>
+      </c>
+      <c r="I44" s="35"/>
+    </row>
+    <row r="45" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <v>176</v>
       </c>
@@ -1462,8 +1960,18 @@
       <c r="E45" s="28">
         <v>59753.59</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F45" s="33">
+        <v>4613.53</v>
+      </c>
+      <c r="G45" s="36">
+        <v>735.84</v>
+      </c>
+      <c r="H45" s="40">
+        <v>1678.3</v>
+      </c>
+      <c r="I45" s="35"/>
+    </row>
+    <row r="46" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
         <v>177</v>
       </c>
@@ -1479,8 +1987,18 @@
       <c r="E46" s="28">
         <v>25394.19</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F46" s="33">
+        <v>4990.12</v>
+      </c>
+      <c r="G46" s="36">
+        <v>877</v>
+      </c>
+      <c r="H46" s="40">
+        <v>1792.75</v>
+      </c>
+      <c r="I46" s="35"/>
+    </row>
+    <row r="47" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A47" s="18">
         <v>178</v>
       </c>
@@ -1496,8 +2014,18 @@
       <c r="E47" s="27">
         <v>1868.29</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F47" s="33">
+        <v>27266.73</v>
+      </c>
+      <c r="G47" s="36">
+        <v>1164.8900000000001</v>
+      </c>
+      <c r="H47" s="40">
+        <v>15818.73</v>
+      </c>
+      <c r="I47" s="35"/>
+    </row>
+    <row r="48" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A48" s="18">
         <v>179</v>
       </c>
@@ -1513,8 +2041,18 @@
       <c r="E48" s="27">
         <v>10402.370000000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F48" s="33">
+        <v>12934.67</v>
+      </c>
+      <c r="G48" s="36">
+        <v>812.04</v>
+      </c>
+      <c r="H48" s="40">
+        <v>9670.2199999999993</v>
+      </c>
+      <c r="I48" s="35"/>
+    </row>
+    <row r="49" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A49" s="18">
         <v>180</v>
       </c>
@@ -1530,8 +2068,18 @@
       <c r="E49" s="27">
         <v>3039.1</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F49" s="33">
+        <v>36582.019999999997</v>
+      </c>
+      <c r="G49" s="36">
+        <v>1346.41</v>
+      </c>
+      <c r="H49" s="40">
+        <v>20135.439999999999</v>
+      </c>
+      <c r="I49" s="35"/>
+    </row>
+    <row r="50" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A50" s="19">
         <v>181</v>
       </c>
@@ -1547,8 +2095,18 @@
       <c r="E50" s="27">
         <v>8726.98</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F50" s="33">
+        <v>1023.06</v>
+      </c>
+      <c r="G50" s="36">
+        <v>279.99</v>
+      </c>
+      <c r="H50" s="40">
+        <v>459.19</v>
+      </c>
+      <c r="I50" s="35"/>
+    </row>
+    <row r="51" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A51" s="19">
         <v>182</v>
       </c>
@@ -1564,8 +2122,18 @@
       <c r="E51" s="28">
         <v>19430.78</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F51" s="33">
+        <v>594.08000000000004</v>
+      </c>
+      <c r="G51" s="36">
+        <v>240.65</v>
+      </c>
+      <c r="H51" s="40">
+        <v>400.71</v>
+      </c>
+      <c r="I51" s="35"/>
+    </row>
+    <row r="52" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="20">
         <v>183</v>
       </c>
@@ -1581,8 +2149,18 @@
       <c r="E52" s="27">
         <v>9342.14</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F52" s="33">
+        <v>1098.44</v>
+      </c>
+      <c r="G52" s="36">
+        <v>296.74</v>
+      </c>
+      <c r="H52" s="40">
+        <v>530.30999999999995</v>
+      </c>
+      <c r="I52" s="35"/>
+    </row>
+    <row r="53" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A53" s="17">
         <v>184</v>
       </c>
@@ -1598,8 +2176,18 @@
       <c r="E53" s="27">
         <v>6712.39</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F53" s="33">
+        <v>1221.06</v>
+      </c>
+      <c r="G53" s="36">
+        <v>150.62</v>
+      </c>
+      <c r="H53" s="40">
+        <v>188.24</v>
+      </c>
+      <c r="I53" s="35"/>
+    </row>
+    <row r="54" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A54" s="14">
         <v>185</v>
       </c>
@@ -1615,8 +2203,18 @@
       <c r="E54" s="28">
         <v>22190.63</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F54" s="33">
+        <v>1552.51</v>
+      </c>
+      <c r="G54" s="36">
+        <v>76.45</v>
+      </c>
+      <c r="H54" s="40">
+        <v>205.76</v>
+      </c>
+      <c r="I54" s="35"/>
+    </row>
+    <row r="55" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A55" s="14">
         <v>186</v>
       </c>
@@ -1632,8 +2230,18 @@
       <c r="E55" s="27">
         <v>12301.49</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F55" s="33">
+        <v>1654.85</v>
+      </c>
+      <c r="G55" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="H55" s="40">
+        <v>335.31</v>
+      </c>
+      <c r="I55" s="35"/>
+    </row>
+    <row r="56" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
         <v>187</v>
       </c>
@@ -1649,8 +2257,18 @@
       <c r="E56" s="28">
         <v>25118.66</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F56" s="33">
+        <v>7708.52</v>
+      </c>
+      <c r="G56" s="36">
+        <v>1319.34</v>
+      </c>
+      <c r="H56" s="40">
+        <v>3564.39</v>
+      </c>
+      <c r="I56" s="35"/>
+    </row>
+    <row r="57" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A57" s="15">
         <v>188</v>
       </c>
@@ -1666,8 +2284,18 @@
       <c r="E57" s="28">
         <v>72143</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F57" s="33">
+        <v>5594.77</v>
+      </c>
+      <c r="G57" s="36">
+        <v>925.84</v>
+      </c>
+      <c r="H57" s="40">
+        <v>2475.23</v>
+      </c>
+      <c r="I57" s="35"/>
+    </row>
+    <row r="58" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A58" s="15">
         <v>189</v>
       </c>
@@ -1683,8 +2311,18 @@
       <c r="E58" s="28">
         <v>41546.61</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F58" s="33">
+        <v>7516.5</v>
+      </c>
+      <c r="G58" s="36">
+        <v>1372.83</v>
+      </c>
+      <c r="H58" s="40">
+        <v>3046.33</v>
+      </c>
+      <c r="I58" s="35"/>
+    </row>
+    <row r="59" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A59" s="18">
         <v>190</v>
       </c>
@@ -1700,8 +2338,18 @@
       <c r="E59" s="27">
         <v>2188</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F59" s="33">
+        <v>18457.38</v>
+      </c>
+      <c r="G59" s="36">
+        <v>1166.69</v>
+      </c>
+      <c r="H59" s="40">
+        <v>13618.9</v>
+      </c>
+      <c r="I59" s="35"/>
+    </row>
+    <row r="60" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A60" s="18">
         <v>191</v>
       </c>
@@ -1717,8 +2365,18 @@
       <c r="E60" s="27">
         <v>11385.68</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F60" s="33">
+        <v>22460.39</v>
+      </c>
+      <c r="G60" s="36">
+        <v>1454.16</v>
+      </c>
+      <c r="H60" s="40">
+        <v>15187.63</v>
+      </c>
+      <c r="I60" s="35"/>
+    </row>
+    <row r="61" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A61" s="18">
         <v>192</v>
       </c>
@@ -1734,8 +2392,18 @@
       <c r="E61" s="27">
         <v>4898.38</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F61" s="33">
+        <v>37394.699999999997</v>
+      </c>
+      <c r="G61" s="36">
+        <v>1122.6500000000001</v>
+      </c>
+      <c r="H61" s="40">
+        <v>22785.5</v>
+      </c>
+      <c r="I61" s="35"/>
+    </row>
+    <row r="62" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A62" s="19">
         <v>193</v>
       </c>
@@ -1751,8 +2419,18 @@
       <c r="E62" s="27">
         <v>8273.4599999999991</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F62" s="33">
+        <v>1225.8699999999999</v>
+      </c>
+      <c r="G62" s="36">
+        <v>183.41</v>
+      </c>
+      <c r="H62" s="40">
+        <v>485.49</v>
+      </c>
+      <c r="I62" s="35"/>
+    </row>
+    <row r="63" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A63" s="19">
         <v>194</v>
       </c>
@@ -1768,8 +2446,18 @@
       <c r="E63" s="28">
         <v>30579.72</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F63" s="33">
+        <v>694.13</v>
+      </c>
+      <c r="G63" s="36">
+        <v>92.15</v>
+      </c>
+      <c r="H63" s="40">
+        <v>174.12</v>
+      </c>
+      <c r="I63" s="35"/>
+    </row>
+    <row r="64" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="20">
         <v>195</v>
       </c>
@@ -1783,8 +2471,18 @@
         <v>43.91</v>
       </c>
       <c r="E64" s="27"/>
-    </row>
-    <row r="65" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F64" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="G64" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="H64" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="I64" s="35"/>
+    </row>
+    <row r="65" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="21">
         <v>196</v>
       </c>
@@ -1798,8 +2496,18 @@
         <v>44.96</v>
       </c>
       <c r="E65" s="27"/>
-    </row>
-    <row r="66" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F65" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G65" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="H65" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="I65" s="35"/>
+    </row>
+    <row r="66" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A66" s="21">
         <v>197</v>
       </c>
@@ -1813,8 +2521,18 @@
         <v>45.73</v>
       </c>
       <c r="E66" s="27"/>
-    </row>
-    <row r="67" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F66" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G66" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="H66" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="I66" s="35"/>
+    </row>
+    <row r="67" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A67" s="14">
         <v>198</v>
       </c>
@@ -1828,8 +2546,18 @@
         <v>41.64</v>
       </c>
       <c r="E67" s="27"/>
-    </row>
-    <row r="68" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F67" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="G67" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="H67" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="I67" s="35"/>
+    </row>
+    <row r="68" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A68" s="14">
         <v>199</v>
       </c>
@@ -1843,8 +2571,18 @@
         <v>44.53</v>
       </c>
       <c r="E68" s="27"/>
-    </row>
-    <row r="69" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F68" s="33">
+        <v>34.270000000000003</v>
+      </c>
+      <c r="G68" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="H68" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="I68" s="35"/>
+    </row>
+    <row r="69" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A69" s="14">
         <v>200</v>
       </c>
@@ -1860,8 +2598,18 @@
       <c r="E69" s="27">
         <v>17303.7</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F69" s="33">
+        <v>1106.94</v>
+      </c>
+      <c r="G69" s="36">
+        <v>267.45</v>
+      </c>
+      <c r="H69" s="40">
+        <v>291.10000000000002</v>
+      </c>
+      <c r="I69" s="35"/>
+    </row>
+    <row r="70" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A70" s="14">
         <v>201</v>
       </c>
@@ -1877,8 +2625,18 @@
       <c r="E70" s="27">
         <v>4653.3500000000004</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F70" s="33">
+        <v>1130.81</v>
+      </c>
+      <c r="G70" s="36">
+        <v>171.79</v>
+      </c>
+      <c r="H70" s="40">
+        <v>310.2</v>
+      </c>
+      <c r="I70" s="35"/>
+    </row>
+    <row r="71" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A71" s="15">
         <v>202</v>
       </c>
@@ -1894,8 +2652,18 @@
       <c r="E71" s="27">
         <v>2593.4</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F71" s="33">
+        <v>1183.2</v>
+      </c>
+      <c r="G71" s="36">
+        <v>162.05000000000001</v>
+      </c>
+      <c r="H71" s="40">
+        <v>277.68</v>
+      </c>
+      <c r="I71" s="35"/>
+    </row>
+    <row r="72" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A72" s="15">
         <v>203</v>
       </c>
@@ -1911,8 +2679,18 @@
       <c r="E72" s="28">
         <v>19340.740000000002</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F72" s="33">
+        <v>2187.36</v>
+      </c>
+      <c r="G72" s="36">
+        <v>169.29</v>
+      </c>
+      <c r="H72" s="40">
+        <v>701.49</v>
+      </c>
+      <c r="I72" s="35"/>
+    </row>
+    <row r="73" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A73" s="15">
         <v>204</v>
       </c>
@@ -1928,8 +2706,18 @@
       <c r="E73" s="27">
         <v>13173.1</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F73" s="33">
+        <v>1162.82</v>
+      </c>
+      <c r="G73" s="36">
+        <v>69.709999999999994</v>
+      </c>
+      <c r="H73" s="40">
+        <v>274.45999999999998</v>
+      </c>
+      <c r="I73" s="35"/>
+    </row>
+    <row r="74" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A74" s="15">
         <v>205</v>
       </c>
@@ -1945,8 +2733,18 @@
       <c r="E74" s="27">
         <v>12673.14</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F74" s="33">
+        <v>2530.87</v>
+      </c>
+      <c r="G74" s="36">
+        <v>497.02</v>
+      </c>
+      <c r="H74" s="40">
+        <v>1165.47</v>
+      </c>
+      <c r="I74" s="35"/>
+    </row>
+    <row r="75" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A75" s="15">
         <v>206</v>
       </c>
@@ -1962,8 +2760,18 @@
       <c r="E75" s="27">
         <v>6484.08</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F75" s="33">
+        <v>1385.53</v>
+      </c>
+      <c r="G75" s="36">
+        <v>132.36000000000001</v>
+      </c>
+      <c r="H75" s="40">
+        <v>337.58</v>
+      </c>
+      <c r="I75" s="35"/>
+    </row>
+    <row r="76" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A76" s="15">
         <v>207</v>
       </c>
@@ -1979,8 +2787,18 @@
       <c r="E76" s="28">
         <v>44838.58</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F76" s="33">
+        <v>13044.71</v>
+      </c>
+      <c r="G76" s="36">
+        <v>1741.25</v>
+      </c>
+      <c r="H76" s="40">
+        <v>3975.24</v>
+      </c>
+      <c r="I76" s="35"/>
+    </row>
+    <row r="77" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A77" s="18">
         <v>208</v>
       </c>
@@ -1996,8 +2814,18 @@
       <c r="E77" s="28">
         <v>1040.74</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F77" s="33">
+        <v>11162.73</v>
+      </c>
+      <c r="G77" s="36">
+        <v>2095.23</v>
+      </c>
+      <c r="H77" s="40">
+        <v>2682.63</v>
+      </c>
+      <c r="I77" s="35"/>
+    </row>
+    <row r="78" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A78" s="18">
         <v>209</v>
       </c>
@@ -2013,8 +2841,18 @@
       <c r="E78" s="28">
         <v>11450.23</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F78" s="33">
+        <v>9588.19</v>
+      </c>
+      <c r="G78" s="36">
+        <v>1094.74</v>
+      </c>
+      <c r="H78" s="40">
+        <v>1529.6</v>
+      </c>
+      <c r="I78" s="35"/>
+    </row>
+    <row r="79" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A79" s="18">
         <v>210</v>
       </c>
@@ -2030,8 +2868,18 @@
       <c r="E79" s="28">
         <v>5335.65</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F79" s="33">
+        <v>7514.72</v>
+      </c>
+      <c r="G79" s="36">
+        <v>1347.54</v>
+      </c>
+      <c r="H79" s="40">
+        <v>1564.2</v>
+      </c>
+      <c r="I79" s="35"/>
+    </row>
+    <row r="80" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A80" s="18">
         <v>211</v>
       </c>
@@ -2047,8 +2895,18 @@
       <c r="E80" s="28">
         <v>11577.23</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F80" s="33">
+        <v>10047.290000000001</v>
+      </c>
+      <c r="G80" s="36">
+        <v>1211.3699999999999</v>
+      </c>
+      <c r="H80" s="40">
+        <v>2223.7399999999998</v>
+      </c>
+      <c r="I80" s="35"/>
+    </row>
+    <row r="81" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A81" s="18">
         <v>212</v>
       </c>
@@ -2064,8 +2922,18 @@
       <c r="E81" s="28">
         <v>29071.9</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F81" s="33">
+        <v>8027.86</v>
+      </c>
+      <c r="G81" s="36">
+        <v>1485.62</v>
+      </c>
+      <c r="H81" s="40">
+        <v>2113.9299999999998</v>
+      </c>
+      <c r="I81" s="35"/>
+    </row>
+    <row r="82" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="22">
         <v>213</v>
       </c>
@@ -2081,8 +2949,18 @@
       <c r="E82" s="27">
         <v>1299.68</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F82" s="33">
+        <v>14357.59</v>
+      </c>
+      <c r="G82" s="36">
+        <v>1190.8699999999999</v>
+      </c>
+      <c r="H82" s="40">
+        <v>10865.44</v>
+      </c>
+      <c r="I82" s="35"/>
+    </row>
+    <row r="83" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A83" s="23">
         <v>220</v>
       </c>
@@ -2098,8 +2976,18 @@
       <c r="E83" s="27">
         <v>8576.93</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F83" s="33">
+        <v>5486.11</v>
+      </c>
+      <c r="G83" s="36">
+        <v>576.42999999999995</v>
+      </c>
+      <c r="H83" s="40">
+        <v>5078.92</v>
+      </c>
+      <c r="I83" s="35"/>
+    </row>
+    <row r="84" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A84" s="23">
         <v>221</v>
       </c>
@@ -2115,8 +3003,18 @@
       <c r="E84" s="27">
         <v>5365.64</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F84" s="33">
+        <v>25850.68</v>
+      </c>
+      <c r="G84" s="36">
+        <v>1125.07</v>
+      </c>
+      <c r="H84" s="40">
+        <v>17967.02</v>
+      </c>
+      <c r="I84" s="35"/>
+    </row>
+    <row r="85" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A85" s="23">
         <v>222</v>
       </c>
@@ -2132,8 +3030,18 @@
       <c r="E85" s="27">
         <v>14836.95</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F85" s="33">
+        <v>2512.94</v>
+      </c>
+      <c r="G85" s="36">
+        <v>50.86</v>
+      </c>
+      <c r="H85" s="40">
+        <v>179.72</v>
+      </c>
+      <c r="I85" s="35"/>
+    </row>
+    <row r="86" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A86" s="23">
         <v>223</v>
       </c>
@@ -2149,8 +3057,18 @@
       <c r="E86" s="28">
         <v>41452.269999999997</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F86" s="33">
+        <v>992.56</v>
+      </c>
+      <c r="G86" s="36">
+        <v>111.05</v>
+      </c>
+      <c r="H86" s="40">
+        <v>209.4</v>
+      </c>
+      <c r="I86" s="35"/>
+    </row>
+    <row r="87" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A87" s="23">
         <v>224</v>
       </c>
@@ -2166,8 +3084,18 @@
       <c r="E87" s="28">
         <v>10659.51</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F87" s="33">
+        <v>745.66</v>
+      </c>
+      <c r="G87" s="36">
+        <v>55</v>
+      </c>
+      <c r="H87" s="40">
+        <v>114.44</v>
+      </c>
+      <c r="I87" s="35"/>
+    </row>
+    <row r="88" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A88" s="23">
         <v>225</v>
       </c>
@@ -2183,8 +3111,18 @@
       <c r="E88" s="27">
         <v>6635.9</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F88" s="33">
+        <v>1250.78</v>
+      </c>
+      <c r="G88" s="36">
+        <v>22.7</v>
+      </c>
+      <c r="H88" s="40">
+        <v>124.13</v>
+      </c>
+      <c r="I88" s="35"/>
+    </row>
+    <row r="89" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="24">
         <v>226</v>
       </c>
@@ -2200,6 +3138,16 @@
       <c r="E89" s="30">
         <v>20781</v>
       </c>
+      <c r="F89" s="33">
+        <v>1202.55</v>
+      </c>
+      <c r="G89" s="36">
+        <v>130.28</v>
+      </c>
+      <c r="H89" s="40">
+        <v>212.68</v>
+      </c>
+      <c r="I89" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>